<commit_message>
converted to rsm my data
</commit_message>
<xml_diff>
--- a/Technical_error_active_learning/src/Manual_CCD_Mg_K_DTT_T7_GFP/analysis_scripts/Darpin_timecourse_ccd1_120723.xlsx
+++ b/Technical_error_active_learning/src/Manual_CCD_Mg_K_DTT_T7_GFP/analysis_scripts/Darpin_timecourse_ccd1_120723.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26707"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26711"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/s1530400_ed_ac_uk/Documents/lab/Plate Reader Data/Timecourse/FDBKps/CCD_Mg_K_DTT_in_lysateE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B377698-64D1-4CAF-A26C-24497A974E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA8471DE-09BD-4619-BD42-D731405618A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="9435" windowHeight="6915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37340,6 +37340,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B418:B421"/>
+    <mergeCell ref="B422:B425"/>
+    <mergeCell ref="B426:B429"/>
+    <mergeCell ref="B430:B433"/>
+    <mergeCell ref="B434:B437"/>
     <mergeCell ref="B438:B441"/>
     <mergeCell ref="B466:B469"/>
     <mergeCell ref="B470:B473"/>
@@ -37351,11 +37356,6 @@
     <mergeCell ref="B454:B457"/>
     <mergeCell ref="B458:B461"/>
     <mergeCell ref="B462:B465"/>
-    <mergeCell ref="B418:B421"/>
-    <mergeCell ref="B422:B425"/>
-    <mergeCell ref="B426:B429"/>
-    <mergeCell ref="B430:B433"/>
-    <mergeCell ref="B434:B437"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -37365,6 +37365,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="344bdced-6c57-4d7b-8a11-5814815f175b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009420611809F90B4D9DF134CBF07160B4" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ed8eb727274b43aef96ed8f147e44d13">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="970d785d-03df-4ab2-9764-c5e22dfeb4bf" xmlns:ns4="344bdced-6c57-4d7b-8a11-5814815f175b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b6e1701f6033d4bc2b489aa651c9e0b9" ns3:_="" ns4:_="">
     <xsd:import namespace="970d785d-03df-4ab2-9764-c5e22dfeb4bf"/>
@@ -37599,14 +37607,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="344bdced-6c57-4d7b-8a11-5814815f175b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -37617,11 +37617,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A68852E5-9D37-4041-83DA-B5CD2C0EB8D3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4D29D4C-8A3B-4999-8B64-791D43262B38}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4D29D4C-8A3B-4999-8B64-791D43262B38}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A68852E5-9D37-4041-83DA-B5CD2C0EB8D3}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>